<commit_message>
Choose language methd is added
</commit_message>
<xml_diff>
--- a/src/test/test_data/Booking.xlsx
+++ b/src/test/test_data/Booking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\Vezba_booking\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0E0ABB-1B3F-4397-BAAE-D71034C1704A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515C1591-9C7F-45FB-BAE2-16DC2C95A3DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Flights" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="68">
   <si>
     <t>tc_id</t>
   </si>
@@ -235,6 +235,12 @@
   </si>
   <si>
     <t>December 2022 15</t>
+  </si>
+  <si>
+    <t>English (UK)</t>
+  </si>
+  <si>
+    <t>language</t>
   </si>
 </sst>
 </file>
@@ -300,7 +306,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -309,16 +315,6 @@
     </fill>
     <fill>
       <gradientFill degree="90">
-        <stop position="0">
-          <color theme="0"/>
-        </stop>
-        <stop position="1">
-          <color theme="9" tint="-0.25098422193060094"/>
-        </stop>
-      </gradientFill>
-    </fill>
-    <fill>
-      <gradientFill>
         <stop position="0">
           <color theme="0"/>
         </stop>
@@ -333,17 +329,17 @@
           <color theme="0"/>
         </stop>
         <stop position="1">
-          <color rgb="FF00B050"/>
+          <color theme="8" tint="0.59999389629810485"/>
         </stop>
       </gradientFill>
     </fill>
     <fill>
-      <gradientFill>
+      <gradientFill degree="90">
         <stop position="0">
           <color theme="0"/>
         </stop>
         <stop position="0.5">
-          <color theme="4" tint="0.40000610370189521"/>
+          <color theme="8" tint="0.59999389629810485"/>
         </stop>
         <stop position="1">
           <color theme="0"/>
@@ -351,7 +347,7 @@
       </gradientFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -525,11 +521,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -541,8 +591,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -551,10 +599,36 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -571,13 +645,10 @@
     <xf numFmtId="49" fontId="7" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -894,10 +965,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1AEBA6-E97B-44CC-BE50-33F6B24023CF}">
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,126 +993,131 @@
     <col min="20" max="20" width="10.28515625" style="1" customWidth="1"/>
     <col min="21" max="21" width="13.85546875" style="1" customWidth="1"/>
     <col min="22" max="22" width="13.7109375" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="1"/>
+    <col min="23" max="23" width="12.85546875" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="24"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="34"/>
     </row>
-    <row r="2" spans="1:22" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
+    <row r="2" spans="1:23" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+    <row r="3" spans="1:23" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="P3" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="Q3" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="R3" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="7" t="s">
+      <c r="S3" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="T3" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="7" t="s">
+      <c r="U3" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="V3" s="8" t="s">
+      <c r="V3" s="27" t="s">
         <v>58</v>
       </c>
+      <c r="W3" s="28" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
@@ -1103,74 +1179,78 @@
         <v>30</v>
       </c>
       <c r="U4" s="4"/>
-      <c r="V4" s="9" t="s">
+      <c r="V4" s="15" t="s">
         <v>35</v>
       </c>
+      <c r="W4" s="7" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="4"/>
-      <c r="P5" s="3" t="s">
+      <c r="O5" s="17"/>
+      <c r="P5" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="Q5" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3" t="s">
+      <c r="R5" s="18"/>
+      <c r="S5" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="T5" s="4" t="s">
+      <c r="T5" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="U5" s="4"/>
-      <c r="V5" s="10"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A1:V1"/>
+    <mergeCell ref="A1:W1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1180,10 +1260,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A940F92-832E-4528-BC43-70A9A766E6BC}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1198,190 +1278,202 @@
     <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
     <col min="9" max="10" width="13.28515625" style="1" customWidth="1"/>
     <col min="11" max="11" width="14" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="12" width="10.85546875" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="27"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
     </row>
-    <row r="2" spans="1:11" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="J3" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="K3" s="18" t="s">
+      <c r="K3" s="23" t="s">
         <v>57</v>
       </c>
+      <c r="L3" s="24" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11" t="s">
+      <c r="I4" s="9"/>
+      <c r="J4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="9" t="s">
         <v>56</v>
       </c>
+      <c r="L4" s="21" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11" t="s">
+      <c r="I5" s="9"/>
+      <c r="J5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="9" t="s">
         <v>43</v>
       </c>
+      <c r="L5" s="8"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="8"/>
     </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="H7" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
One-way flight scenario is added
</commit_message>
<xml_diff>
--- a/src/test/test_data/Booking.xlsx
+++ b/src/test/test_data/Booking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\Vezba_booking\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515C1591-9C7F-45FB-BAE2-16DC2C95A3DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D91586-CF1B-4121-A225-3C6325B1D880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Flights" sheetId="1" r:id="rId1"/>
@@ -168,9 +168,6 @@
     <t>numRooms</t>
   </si>
   <si>
-    <t>Kopaonik</t>
-  </si>
-  <si>
     <t>17 15</t>
   </si>
   <si>
@@ -207,9 +204,6 @@
     <t>November 2022 17</t>
   </si>
   <si>
-    <t>Kikinda</t>
-  </si>
-  <si>
     <t>verifResults</t>
   </si>
   <si>
@@ -241,6 +235,12 @@
   </si>
   <si>
     <t>language</t>
+  </si>
+  <si>
+    <t>Belgrade</t>
+  </si>
+  <si>
+    <t>Zagreb</t>
   </si>
 </sst>
 </file>
@@ -967,7 +967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1AEBA6-E97B-44CC-BE50-33F6B24023CF}">
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -1111,10 +1111,10 @@
         <v>34</v>
       </c>
       <c r="V3" s="27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="W3" s="28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
@@ -1128,34 +1128,34 @@
         <v>22</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>24</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="I4" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>27</v>
@@ -1164,16 +1164,16 @@
         <v>28</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R4" s="4" t="s">
         <v>29</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="T4" s="4" t="s">
         <v>30</v>
@@ -1183,7 +1183,7 @@
         <v>35</v>
       </c>
       <c r="W4" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1200,45 +1200,45 @@
         <v>23</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>24</v>
       </c>
       <c r="G5" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="18" t="s">
-        <v>61</v>
-      </c>
       <c r="I5" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J5" s="17" t="s">
         <v>25</v>
       </c>
       <c r="K5" s="18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L5" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M5" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N5" s="17" t="s">
         <v>27</v>
       </c>
       <c r="O5" s="17"/>
       <c r="P5" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Q5" s="18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R5" s="18"/>
       <c r="S5" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="T5" s="17" t="s">
         <v>30</v>
@@ -1262,8 +1262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A940F92-832E-4528-BC43-70A9A766E6BC}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1330,27 +1330,27 @@
         <v>34</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K3" s="23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L3" s="24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>21</v>
@@ -1359,7 +1359,7 @@
         <v>32</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>32</v>
@@ -1369,24 +1369,24 @@
         <v>35</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="L4" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>32</v>
@@ -1395,7 +1395,7 @@
         <v>32</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>32</v>
@@ -1405,22 +1405,22 @@
         <v>35</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="L5" s="8"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>32</v>
@@ -1429,7 +1429,7 @@
         <v>21</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H6" s="10" t="s">
         <v>32</v>
@@ -1441,28 +1441,28 @@
     </row>
     <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>32</v>
       </c>
       <c r="F7" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="14" t="s">
-        <v>47</v>
-      </c>
       <c r="H7" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>

</xml_diff>

<commit_message>
booking xlsx file is udpated
</commit_message>
<xml_diff>
--- a/src/test/test_data/Booking.xlsx
+++ b/src/test/test_data/Booking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\Vezba_booking\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D91586-CF1B-4121-A225-3C6325B1D880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F7314E-D892-49F9-A7B9-CA091C6286AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Flights" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="84">
   <si>
     <t>tc_id</t>
   </si>
@@ -241,6 +241,54 @@
   </si>
   <si>
     <t>Zagreb</t>
+  </si>
+  <si>
+    <t>flightClass1</t>
+  </si>
+  <si>
+    <t>flightClass2</t>
+  </si>
+  <si>
+    <t>flightClass3</t>
+  </si>
+  <si>
+    <t>flightClass4</t>
+  </si>
+  <si>
+    <t>ECONOMY</t>
+  </si>
+  <si>
+    <t>BUSINESS</t>
+  </si>
+  <si>
+    <t>expectedFlightClass1</t>
+  </si>
+  <si>
+    <t>expectedFlightClass2</t>
+  </si>
+  <si>
+    <t>expectedFlightClass3</t>
+  </si>
+  <si>
+    <t>expectedFlightClass4</t>
+  </si>
+  <si>
+    <t>Economy</t>
+  </si>
+  <si>
+    <t>Premium economy</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>First class</t>
+  </si>
+  <si>
+    <t>PREMIUM_ECONOMY</t>
+  </si>
+  <si>
+    <t>FIRST_CLASS</t>
   </si>
 </sst>
 </file>
@@ -347,7 +395,7 @@
       </gradientFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -455,43 +503,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -579,7 +590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -591,28 +602,27 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -621,28 +631,32 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -965,10 +979,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1AEBA6-E97B-44CC-BE50-33F6B24023CF}">
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:AE5"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,130 +1008,164 @@
     <col min="21" max="21" width="13.85546875" style="1" customWidth="1"/>
     <col min="22" max="22" width="13.7109375" style="1" customWidth="1"/>
     <col min="23" max="23" width="12.85546875" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="1"/>
+    <col min="24" max="24" width="11.42578125" style="1" customWidth="1"/>
+    <col min="25" max="27" width="11.28515625" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="35"/>
+      <c r="AB1" s="35"/>
+      <c r="AC1" s="35"/>
+      <c r="AD1" s="35"/>
+      <c r="AE1" s="35"/>
     </row>
-    <row r="2" spans="1:23" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
+    <row r="2" spans="1:31" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
     </row>
-    <row r="3" spans="1:23" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+    <row r="3" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="I3" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="26" t="s">
+      <c r="K3" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="26" t="s">
+      <c r="L3" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="26" t="s">
+      <c r="M3" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="26" t="s">
+      <c r="N3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="26" t="s">
+      <c r="O3" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="26" t="s">
+      <c r="P3" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="26" t="s">
+      <c r="Q3" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="26" t="s">
+      <c r="R3" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="26" t="s">
+      <c r="S3" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="26" t="s">
+      <c r="T3" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="26" t="s">
+      <c r="U3" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="V3" s="27" t="s">
+      <c r="V3" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="W3" s="28" t="s">
+      <c r="W3" s="27" t="s">
         <v>65</v>
       </c>
+      <c r="X3" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y3" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z3" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA3" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB3" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC3" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD3" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE3" s="27" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" ht="39" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
@@ -1179,78 +1227,110 @@
         <v>30</v>
       </c>
       <c r="U4" s="4"/>
-      <c r="V4" s="15" t="s">
+      <c r="V4" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="W4" s="7" t="s">
+      <c r="W4" s="30" t="s">
         <v>64</v>
       </c>
+      <c r="X4" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y4" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z4" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA4" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB4" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC4" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD4" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE4" s="31" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="I5" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="18" t="s">
+      <c r="K5" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="L5" s="18" t="s">
+      <c r="L5" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="M5" s="18" t="s">
+      <c r="M5" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="N5" s="17" t="s">
+      <c r="N5" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="17"/>
-      <c r="P5" s="18" t="s">
+      <c r="O5" s="16"/>
+      <c r="P5" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="Q5" s="18" t="s">
+      <c r="Q5" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="R5" s="18"/>
-      <c r="S5" s="18" t="s">
+      <c r="R5" s="17"/>
+      <c r="S5" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="T5" s="17" t="s">
+      <c r="T5" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="U5" s="17"/>
-      <c r="V5" s="19"/>
-      <c r="W5" s="20"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="18"/>
+      <c r="W5" s="29"/>
+      <c r="X5" s="29"/>
+      <c r="Y5" s="29"/>
+      <c r="Z5" s="29"/>
+      <c r="AA5" s="19"/>
+      <c r="AB5" s="29"/>
+      <c r="AC5" s="29"/>
+      <c r="AD5" s="29"/>
+      <c r="AE5" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A1:W1"/>
+    <mergeCell ref="A1:AE1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1262,7 +1342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A940F92-832E-4528-BC43-70A9A766E6BC}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
@@ -1283,191 +1363,191 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
     </row>
     <row r="2" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="J3" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="K3" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="L3" s="24" t="s">
+      <c r="L3" s="23" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9" t="s">
+      <c r="I4" s="8"/>
+      <c r="J4" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="L4" s="21" t="s">
+      <c r="L4" s="20" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9" t="s">
+      <c r="I5" s="8"/>
+      <c r="J5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="L5" s="8"/>
+      <c r="L5" s="7"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="7"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="20"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Cars Rental page is added
</commit_message>
<xml_diff>
--- a/src/test/test_data/Booking.xlsx
+++ b/src/test/test_data/Booking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\Vezba_booking\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED73C8C4-CA41-417B-8553-9572C36964BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCA98C7-A706-4DC0-A10B-715F59E022A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-1905" yWindow="-13050" windowWidth="22950" windowHeight="7875" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Flights" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="97">
   <si>
     <t>tc_id</t>
   </si>
@@ -315,13 +315,19 @@
     <t>19</t>
   </si>
   <si>
-    <t>Milan</t>
-  </si>
-  <si>
     <t xml:space="preserve">We can’t find any flights </t>
   </si>
   <si>
     <t>expectedTextFirstClass</t>
+  </si>
+  <si>
+    <t>Skopje</t>
+  </si>
+  <si>
+    <t>urlCarPage</t>
+  </si>
+  <si>
+    <t>car</t>
   </si>
 </sst>
 </file>
@@ -966,10 +972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1AEBA6-E97B-44CC-BE50-33F6B24023CF}">
-  <dimension ref="A1:AG6"/>
+  <dimension ref="A1:AH6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,21 +1000,21 @@
     <col min="18" max="19" width="9.140625" style="1"/>
     <col min="20" max="20" width="10.28515625" style="1" customWidth="1"/>
     <col min="21" max="21" width="13.85546875" style="1" customWidth="1"/>
-    <col min="22" max="22" width="13.7109375" style="1" customWidth="1"/>
-    <col min="23" max="23" width="12.85546875" style="1" customWidth="1"/>
-    <col min="24" max="24" width="11.42578125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="17.42578125" style="1" customWidth="1"/>
-    <col min="26" max="27" width="11.28515625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="21" style="1" customWidth="1"/>
-    <col min="29" max="29" width="22" style="1" customWidth="1"/>
-    <col min="30" max="30" width="21" style="1" customWidth="1"/>
-    <col min="31" max="31" width="20.85546875" style="1" customWidth="1"/>
-    <col min="32" max="32" width="37.7109375" style="1" customWidth="1"/>
-    <col min="33" max="33" width="24" style="1" customWidth="1"/>
-    <col min="34" max="16384" width="9.140625" style="1"/>
+    <col min="22" max="23" width="13.7109375" style="1" customWidth="1"/>
+    <col min="24" max="24" width="12.85546875" style="1" customWidth="1"/>
+    <col min="25" max="25" width="11.42578125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="17.42578125" style="1" customWidth="1"/>
+    <col min="27" max="28" width="11.28515625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="21" style="1" customWidth="1"/>
+    <col min="30" max="30" width="22" style="1" customWidth="1"/>
+    <col min="31" max="31" width="21" style="1" customWidth="1"/>
+    <col min="32" max="32" width="20.85546875" style="1" customWidth="1"/>
+    <col min="33" max="33" width="37.7109375" style="1" customWidth="1"/>
+    <col min="34" max="34" width="24" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>32</v>
       </c>
@@ -1044,8 +1050,9 @@
       <c r="AE1" s="26"/>
       <c r="AF1" s="26"/>
       <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
     </row>
-    <row r="2" spans="1:33" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -1067,7 +1074,7 @@
       <c r="S2" s="24"/>
       <c r="T2" s="24"/>
     </row>
-    <row r="3" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -1135,40 +1142,43 @@
         <v>55</v>
       </c>
       <c r="W3" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="X3" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="X3" s="10" t="s">
+      <c r="Y3" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="Y3" s="10" t="s">
+      <c r="Z3" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="Z3" s="10" t="s">
+      <c r="AA3" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="AA3" s="10" t="s">
+      <c r="AB3" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="AB3" s="10" t="s">
+      <c r="AC3" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="AC3" s="10" t="s">
+      <c r="AD3" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="AD3" s="10" t="s">
+      <c r="AE3" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="AE3" s="10" t="s">
+      <c r="AF3" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="AF3" s="10" t="s">
+      <c r="AG3" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="AG3" s="10" t="s">
-        <v>94</v>
+      <c r="AH3" s="10" t="s">
+        <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -1233,41 +1243,44 @@
       <c r="V4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="W4" s="8" t="s">
+      <c r="W4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="X4" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="X4" s="8" t="s">
+      <c r="Y4" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="Y4" s="8" t="s">
+      <c r="Z4" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="Z4" s="8" t="s">
+      <c r="AA4" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="AA4" s="8" t="s">
+      <c r="AB4" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="AB4" s="8" t="s">
+      <c r="AC4" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="AC4" s="8" t="s">
+      <c r="AD4" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="AD4" s="8" t="s">
+      <c r="AE4" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AE4" s="8" t="s">
+      <c r="AF4" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="AF4" s="8" t="s">
+      <c r="AG4" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="AG4" s="11" t="s">
-        <v>93</v>
+      <c r="AH4" s="11" t="s">
+        <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
@@ -1326,7 +1339,9 @@
       </c>
       <c r="U5" s="4"/>
       <c r="V5" s="11"/>
-      <c r="W5" s="11"/>
+      <c r="W5" s="11" t="s">
+        <v>96</v>
+      </c>
       <c r="X5" s="11"/>
       <c r="Y5" s="11"/>
       <c r="Z5" s="11"/>
@@ -1337,8 +1352,9 @@
       <c r="AE5" s="11"/>
       <c r="AF5" s="11"/>
       <c r="AG5" s="11"/>
+      <c r="AH5" s="11"/>
     </row>
-    <row r="6" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>89</v>
       </c>
@@ -1346,7 +1362,7 @@
         <v>44</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>85</v>
@@ -1403,42 +1419,47 @@
       <c r="V6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="W6" s="8" t="s">
+      <c r="W6" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="X6" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="X6" s="8" t="s">
+      <c r="Y6" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="Y6" s="8" t="s">
+      <c r="Z6" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="Z6" s="8" t="s">
+      <c r="AA6" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="AA6" s="8" t="s">
+      <c r="AB6" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="AB6" s="8" t="s">
+      <c r="AC6" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="AC6" s="8" t="s">
+      <c r="AD6" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="AD6" s="8" t="s">
+      <c r="AE6" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AE6" s="8" t="s">
+      <c r="AF6" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="AF6" s="8" t="s">
+      <c r="AG6" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="AG6" s="11"/>
+      <c r="AH6" s="11" t="s">
+        <v>92</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A1:AG1"/>
+    <mergeCell ref="A1:AH1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
final commit - complete
</commit_message>
<xml_diff>
--- a/src/test/test_data/Booking.xlsx
+++ b/src/test/test_data/Booking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\Vezba_booking\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCA98C7-A706-4DC0-A10B-715F59E022A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6302806-A77D-41DE-9256-08AC35162144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1905" yWindow="-13050" windowWidth="22950" windowHeight="7875" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Flights" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="101">
   <si>
     <t>tc_id</t>
   </si>
@@ -328,6 +328,18 @@
   </si>
   <si>
     <t>car</t>
+  </si>
+  <si>
+    <t>FL_004</t>
+  </si>
+  <si>
+    <t>Fri 20 Jan</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Wed 25 Jan</t>
   </si>
 </sst>
 </file>
@@ -972,10 +984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1AEBA6-E97B-44CC-BE50-33F6B24023CF}">
-  <dimension ref="A1:AH6"/>
+  <dimension ref="A1:AH7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AH14" sqref="AH14:AH15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,6 +1468,108 @@
         <v>92</v>
       </c>
     </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="U7" s="4"/>
+      <c r="V7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="X7" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y7" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z7" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA7" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB7" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC7" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD7" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE7" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF7" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG7" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH7" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:T2"/>

</xml_diff>

<commit_message>
passnger choise is added
</commit_message>
<xml_diff>
--- a/src/test/test_data/Booking.xlsx
+++ b/src/test/test_data/Booking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\Vezba_booking\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6302806-A77D-41DE-9256-08AC35162144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBB93CE-C7D0-4789-860F-46FFC6ECA50B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="113">
   <si>
     <t>tc_id</t>
   </si>
@@ -333,13 +333,49 @@
     <t>FL_004</t>
   </si>
   <si>
-    <t>Fri 20 Jan</t>
-  </si>
-  <si>
     <t>25</t>
   </si>
   <si>
-    <t>Wed 25 Jan</t>
+    <t>Wed 30 Nov</t>
+  </si>
+  <si>
+    <t>Fri 25 Nov</t>
+  </si>
+  <si>
+    <t>November 2022</t>
+  </si>
+  <si>
+    <t>TC_005</t>
+  </si>
+  <si>
+    <t>numAdultsFlight</t>
+  </si>
+  <si>
+    <t>numChildrenFlight</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>childrenAgesFlight</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>8 9 10 11</t>
+  </si>
+  <si>
+    <t>12 13 14</t>
+  </si>
+  <si>
+    <t>8 9</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -454,7 +490,7 @@
       </gradientFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -606,11 +642,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -619,7 +692,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -652,6 +724,10 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -664,10 +740,13 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -984,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1AEBA6-E97B-44CC-BE50-33F6B24023CF}">
-  <dimension ref="A1:AH7"/>
+  <dimension ref="A1:AK7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AH14" sqref="AH14:AH15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,193 +1083,208 @@
     <col min="10" max="10" width="5.85546875" style="1" customWidth="1"/>
     <col min="11" max="11" width="15.28515625" style="1" customWidth="1"/>
     <col min="12" max="12" width="16.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="1"/>
+    <col min="13" max="13" width="14.85546875" style="1" customWidth="1"/>
     <col min="14" max="14" width="5.7109375" style="1" customWidth="1"/>
     <col min="15" max="15" width="15.140625" style="1" customWidth="1"/>
     <col min="16" max="16" width="16.42578125" style="1" customWidth="1"/>
     <col min="17" max="17" width="13.42578125" style="1" customWidth="1"/>
-    <col min="18" max="19" width="9.140625" style="1"/>
+    <col min="18" max="18" width="9.140625" style="1"/>
+    <col min="19" max="19" width="13.28515625" style="1" customWidth="1"/>
     <col min="20" max="20" width="10.28515625" style="1" customWidth="1"/>
     <col min="21" max="21" width="13.85546875" style="1" customWidth="1"/>
     <col min="22" max="23" width="13.7109375" style="1" customWidth="1"/>
     <col min="24" max="24" width="12.85546875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="11.42578125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="17.42578125" style="1" customWidth="1"/>
-    <col min="27" max="28" width="11.28515625" style="1" customWidth="1"/>
-    <col min="29" max="29" width="21" style="1" customWidth="1"/>
-    <col min="30" max="30" width="22" style="1" customWidth="1"/>
-    <col min="31" max="31" width="21" style="1" customWidth="1"/>
-    <col min="32" max="32" width="20.85546875" style="1" customWidth="1"/>
-    <col min="33" max="33" width="37.7109375" style="1" customWidth="1"/>
-    <col min="34" max="34" width="24" style="1" customWidth="1"/>
-    <col min="35" max="16384" width="9.140625" style="1"/>
+    <col min="25" max="25" width="15.7109375" style="1" customWidth="1"/>
+    <col min="26" max="27" width="18" style="1" customWidth="1"/>
+    <col min="28" max="28" width="11.42578125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="17.42578125" style="1" customWidth="1"/>
+    <col min="30" max="31" width="11.28515625" style="1" customWidth="1"/>
+    <col min="32" max="32" width="21" style="1" customWidth="1"/>
+    <col min="33" max="33" width="22" style="1" customWidth="1"/>
+    <col min="34" max="34" width="21" style="1" customWidth="1"/>
+    <col min="35" max="35" width="20.85546875" style="1" customWidth="1"/>
+    <col min="36" max="36" width="37.7109375" style="1" customWidth="1"/>
+    <col min="37" max="37" width="24" style="1" customWidth="1"/>
+    <col min="38" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="26"/>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26"/>
-      <c r="AB1" s="26"/>
-      <c r="AC1" s="26"/>
-      <c r="AD1" s="26"/>
-      <c r="AE1" s="26"/>
-      <c r="AF1" s="26"/>
-      <c r="AG1" s="26"/>
-      <c r="AH1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="27"/>
+      <c r="AG1" s="27"/>
+      <c r="AH1" s="27"/>
+      <c r="AI1" s="27"/>
+      <c r="AJ1" s="27"/>
+      <c r="AK1" s="27"/>
     </row>
-    <row r="2" spans="1:34" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
+    <row r="2" spans="1:37" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
     </row>
-    <row r="3" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:37" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="O3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="P3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="Q3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="10" t="s">
+      <c r="R3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="10" t="s">
+      <c r="S3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="10" t="s">
+      <c r="T3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="10" t="s">
+      <c r="U3" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="V3" s="10" t="s">
+      <c r="V3" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="W3" s="10" t="s">
+      <c r="W3" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="X3" s="10" t="s">
+      <c r="X3" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="Y3" s="10" t="s">
+      <c r="Y3" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z3" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA3" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB3" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="Z3" s="10" t="s">
+      <c r="AC3" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="AA3" s="10" t="s">
+      <c r="AD3" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="AB3" s="10" t="s">
+      <c r="AE3" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="AC3" s="10" t="s">
+      <c r="AF3" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="AD3" s="10" t="s">
+      <c r="AG3" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="AE3" s="10" t="s">
+      <c r="AH3" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="AF3" s="10" t="s">
+      <c r="AI3" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="AG3" s="10" t="s">
+      <c r="AJ3" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="AH3" s="10" t="s">
+      <c r="AK3" s="9" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -1258,41 +1352,50 @@
       <c r="W4" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="X4" s="8" t="s">
+      <c r="X4" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="Y4" s="8" t="s">
+      <c r="Y4" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z4" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA4" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB4" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="Z4" s="8" t="s">
+      <c r="AC4" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="AA4" s="8" t="s">
+      <c r="AD4" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AB4" s="8" t="s">
+      <c r="AE4" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="AC4" s="8" t="s">
+      <c r="AF4" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="AD4" s="8" t="s">
+      <c r="AG4" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="AE4" s="8" t="s">
+      <c r="AH4" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="AF4" s="8" t="s">
+      <c r="AI4" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="AG4" s="8" t="s">
+      <c r="AJ4" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="AH4" s="11" t="s">
+      <c r="AK4" s="10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
@@ -1350,23 +1453,32 @@
         <v>29</v>
       </c>
       <c r="U5" s="4"/>
-      <c r="V5" s="11"/>
-      <c r="W5" s="11" t="s">
+      <c r="V5" s="10"/>
+      <c r="W5" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="11"/>
-      <c r="Z5" s="11"/>
-      <c r="AA5" s="11"/>
-      <c r="AB5" s="11"/>
-      <c r="AC5" s="11"/>
-      <c r="AD5" s="11"/>
-      <c r="AE5" s="11"/>
-      <c r="AF5" s="11"/>
-      <c r="AG5" s="11"/>
-      <c r="AH5" s="11"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA5" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB5" s="10"/>
+      <c r="AC5" s="10"/>
+      <c r="AD5" s="10"/>
+      <c r="AE5" s="10"/>
+      <c r="AF5" s="10"/>
+      <c r="AG5" s="10"/>
+      <c r="AH5" s="10"/>
+      <c r="AI5" s="10"/>
+      <c r="AJ5" s="10"/>
+      <c r="AK5" s="10"/>
     </row>
-    <row r="6" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>89</v>
       </c>
@@ -1434,41 +1546,50 @@
       <c r="W6" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="X6" s="8" t="s">
+      <c r="X6" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="Y6" s="8" t="s">
+      <c r="Y6" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z6" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA6" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB6" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="Z6" s="8" t="s">
+      <c r="AC6" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="AA6" s="8" t="s">
+      <c r="AD6" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AB6" s="8" t="s">
+      <c r="AE6" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="AC6" s="8" t="s">
+      <c r="AF6" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="AD6" s="8" t="s">
+      <c r="AG6" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="AE6" s="8" t="s">
+      <c r="AH6" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="AF6" s="8" t="s">
+      <c r="AI6" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="AG6" s="8" t="s">
+      <c r="AJ6" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="AH6" s="11" t="s">
+      <c r="AK6" s="10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>97</v>
       </c>
@@ -1506,13 +1627,13 @@
         <v>56</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>26</v>
+        <v>98</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="P7" s="3" t="s">
         <v>56</v>
@@ -1521,13 +1642,13 @@
         <v>60</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>99</v>
+        <v>29</v>
       </c>
       <c r="U7" s="4"/>
       <c r="V7" s="3" t="s">
@@ -1536,44 +1657,53 @@
       <c r="W7" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="X7" s="8" t="s">
+      <c r="X7" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="Y7" s="8" t="s">
+      <c r="Y7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA7" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB7" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="Z7" s="8" t="s">
+      <c r="AC7" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="AA7" s="8" t="s">
+      <c r="AD7" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AB7" s="8" t="s">
+      <c r="AE7" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="AC7" s="8" t="s">
+      <c r="AF7" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="AD7" s="8" t="s">
+      <c r="AG7" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="AE7" s="8" t="s">
+      <c r="AH7" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="AF7" s="8" t="s">
+      <c r="AI7" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="AG7" s="8" t="s">
+      <c r="AJ7" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="AH7" s="11" t="s">
+      <c r="AK7" s="10" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A1:AH1"/>
+    <mergeCell ref="A1:AK1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1583,10 +1713,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A940F92-832E-4528-BC43-70A9A766E6BC}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1605,194 +1735,230 @@
     <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="30"/>
     </row>
     <row r="2" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
+      <c r="A2" s="21"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="L3" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16" t="s">
+      <c r="I4" s="15"/>
+      <c r="J4" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="K4" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="L4" s="18" t="s">
+      <c r="L4" s="17" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16" t="s">
+      <c r="I5" s="15"/>
+      <c r="J5" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="L5" s="18" t="s">
+      <c r="L5" s="17" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="19" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="6"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="L8" s="22" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Car rentals: pickup and dropoff time methods are added
</commit_message>
<xml_diff>
--- a/src/test/test_data/Booking.xlsx
+++ b/src/test/test_data/Booking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\Vezba_booking\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6302806-A77D-41DE-9256-08AC35162144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D1FDC0-A5D0-449D-AA56-8D96C9ADF92A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="113">
   <si>
     <t>tc_id</t>
   </si>
@@ -336,10 +336,46 @@
     <t>Fri 20 Jan</t>
   </si>
   <si>
+    <t>Wed 25 Jan</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
     <t>25</t>
   </si>
   <si>
-    <t>Wed 25 Jan</t>
+    <t>29</t>
+  </si>
+  <si>
+    <t>pickupHour</t>
+  </si>
+  <si>
+    <t>pickupMinutes</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>dropHour</t>
+  </si>
+  <si>
+    <t>dropMinutes</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
   </si>
 </sst>
 </file>
@@ -610,7 +646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -652,6 +688,10 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -984,10 +1024,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1AEBA6-E97B-44CC-BE50-33F6B24023CF}">
-  <dimension ref="A1:AH7"/>
+  <dimension ref="A1:AL7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AH14" sqref="AH14:AH15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AC13" sqref="AC13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,80 +1053,87 @@
     <col min="20" max="20" width="10.28515625" style="1" customWidth="1"/>
     <col min="21" max="21" width="13.85546875" style="1" customWidth="1"/>
     <col min="22" max="23" width="13.7109375" style="1" customWidth="1"/>
-    <col min="24" max="24" width="12.85546875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="11.42578125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="17.42578125" style="1" customWidth="1"/>
-    <col min="27" max="28" width="11.28515625" style="1" customWidth="1"/>
-    <col min="29" max="29" width="21" style="1" customWidth="1"/>
-    <col min="30" max="30" width="22" style="1" customWidth="1"/>
-    <col min="31" max="31" width="21" style="1" customWidth="1"/>
-    <col min="32" max="32" width="20.85546875" style="1" customWidth="1"/>
-    <col min="33" max="33" width="37.7109375" style="1" customWidth="1"/>
-    <col min="34" max="34" width="24" style="1" customWidth="1"/>
-    <col min="35" max="16384" width="9.140625" style="1"/>
+    <col min="24" max="25" width="12.85546875" style="1" customWidth="1"/>
+    <col min="26" max="26" width="15" style="1" customWidth="1"/>
+    <col min="27" max="27" width="11" style="1" customWidth="1"/>
+    <col min="28" max="28" width="12.42578125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="11.42578125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="17.42578125" style="1" customWidth="1"/>
+    <col min="31" max="32" width="11.28515625" style="1" customWidth="1"/>
+    <col min="33" max="33" width="21" style="1" customWidth="1"/>
+    <col min="34" max="34" width="22" style="1" customWidth="1"/>
+    <col min="35" max="35" width="21" style="1" customWidth="1"/>
+    <col min="36" max="36" width="20.85546875" style="1" customWidth="1"/>
+    <col min="37" max="37" width="37.7109375" style="1" customWidth="1"/>
+    <col min="38" max="38" width="24" style="1" customWidth="1"/>
+    <col min="39" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:38" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="26"/>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26"/>
-      <c r="AB1" s="26"/>
-      <c r="AC1" s="26"/>
-      <c r="AD1" s="26"/>
-      <c r="AE1" s="26"/>
-      <c r="AF1" s="26"/>
-      <c r="AG1" s="26"/>
-      <c r="AH1" s="26"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="28"/>
+      <c r="AG1" s="28"/>
+      <c r="AH1" s="28"/>
+      <c r="AI1" s="28"/>
+      <c r="AJ1" s="28"/>
+      <c r="AK1" s="28"/>
+      <c r="AL1" s="28"/>
     </row>
-    <row r="2" spans="1:34" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
+    <row r="2" spans="1:38" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
     </row>
-    <row r="3" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -1160,37 +1207,49 @@
         <v>64</v>
       </c>
       <c r="Y3" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z3" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA3" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB3" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC3" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="Z3" s="10" t="s">
+      <c r="AD3" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="AA3" s="10" t="s">
+      <c r="AE3" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="AB3" s="10" t="s">
+      <c r="AF3" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="AC3" s="10" t="s">
+      <c r="AG3" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="AD3" s="10" t="s">
+      <c r="AH3" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="AE3" s="10" t="s">
+      <c r="AI3" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="AF3" s="10" t="s">
+      <c r="AJ3" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="AG3" s="10" t="s">
+      <c r="AK3" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="AH3" s="10" t="s">
+      <c r="AL3" s="10" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -1261,38 +1320,50 @@
       <c r="X4" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="Y4" s="8" t="s">
+      <c r="Y4" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z4" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA4" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB4" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC4" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="Z4" s="8" t="s">
+      <c r="AD4" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="AA4" s="8" t="s">
+      <c r="AE4" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="AB4" s="8" t="s">
+      <c r="AF4" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="AC4" s="8" t="s">
+      <c r="AG4" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="AD4" s="8" t="s">
+      <c r="AH4" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="AE4" s="8" t="s">
+      <c r="AI4" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AF4" s="8" t="s">
+      <c r="AJ4" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="AG4" s="8" t="s">
+      <c r="AK4" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="AH4" s="11" t="s">
+      <c r="AL4" s="11" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
@@ -1355,18 +1426,30 @@
         <v>96</v>
       </c>
       <c r="X5" s="11"/>
-      <c r="Y5" s="11"/>
-      <c r="Z5" s="11"/>
-      <c r="AA5" s="11"/>
-      <c r="AB5" s="11"/>
+      <c r="Y5" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z5" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA5" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB5" s="24" t="s">
+        <v>25</v>
+      </c>
       <c r="AC5" s="11"/>
       <c r="AD5" s="11"/>
       <c r="AE5" s="11"/>
       <c r="AF5" s="11"/>
       <c r="AG5" s="11"/>
       <c r="AH5" s="11"/>
+      <c r="AI5" s="11"/>
+      <c r="AJ5" s="11"/>
+      <c r="AK5" s="11"/>
+      <c r="AL5" s="11"/>
     </row>
-    <row r="6" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>89</v>
       </c>
@@ -1437,38 +1520,50 @@
       <c r="X6" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="Y6" s="8" t="s">
+      <c r="Y6" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z6" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA6" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB6" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC6" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="Z6" s="8" t="s">
+      <c r="AD6" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="AA6" s="8" t="s">
+      <c r="AE6" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="AB6" s="8" t="s">
+      <c r="AF6" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="AC6" s="8" t="s">
+      <c r="AG6" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="AD6" s="8" t="s">
+      <c r="AH6" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="AE6" s="8" t="s">
+      <c r="AI6" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AF6" s="8" t="s">
+      <c r="AJ6" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="AG6" s="8" t="s">
+      <c r="AK6" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="AH6" s="11" t="s">
+      <c r="AL6" s="11" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>97</v>
       </c>
@@ -1505,11 +1600,11 @@
       <c r="L7" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="M7" s="3" t="s">
-        <v>57</v>
+      <c r="M7" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>26</v>
+        <v>101</v>
       </c>
       <c r="O7" s="4" t="s">
         <v>98</v>
@@ -1521,13 +1616,13 @@
         <v>60</v>
       </c>
       <c r="R7" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="S7" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="S7" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="T7" s="4" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="U7" s="4"/>
       <c r="V7" s="3" t="s">
@@ -1539,41 +1634,53 @@
       <c r="X7" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="Y7" s="8" t="s">
+      <c r="Y7" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z7" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA7" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB7" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC7" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="Z7" s="8" t="s">
+      <c r="AD7" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="AA7" s="8" t="s">
+      <c r="AE7" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="AB7" s="8" t="s">
+      <c r="AF7" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="AC7" s="8" t="s">
+      <c r="AG7" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="AD7" s="8" t="s">
+      <c r="AH7" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="AE7" s="8" t="s">
+      <c r="AI7" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AF7" s="8" t="s">
+      <c r="AJ7" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="AG7" s="8" t="s">
+      <c r="AK7" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="AH7" s="11" t="s">
+      <c r="AL7" s="11" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A1:AH1"/>
+    <mergeCell ref="A1:AL1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1606,20 +1713,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
     </row>
     <row r="2" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22"/>

</xml_diff>

<commit_message>
parallel way for execution is exapnded
</commit_message>
<xml_diff>
--- a/src/test/test_data/Booking.xlsx
+++ b/src/test/test_data/Booking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\Vezba_booking\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBB93CE-C7D0-4789-860F-46FFC6ECA50B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484F1CEF-0637-4202-9A80-AEE4216C0B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Flights" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="121">
   <si>
     <t>tc_id</t>
   </si>
@@ -376,6 +376,30 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>pickupHour</t>
+  </si>
+  <si>
+    <t>pickupMinutes</t>
+  </si>
+  <si>
+    <t>dropHour</t>
+  </si>
+  <si>
+    <t>dropMinutes</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
   </si>
 </sst>
 </file>
@@ -1063,10 +1087,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1AEBA6-E97B-44CC-BE50-33F6B24023CF}">
-  <dimension ref="A1:AK7"/>
+  <dimension ref="A1:AO7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="AD15" sqref="AD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,22 +1117,24 @@
     <col min="20" max="20" width="10.28515625" style="1" customWidth="1"/>
     <col min="21" max="21" width="13.85546875" style="1" customWidth="1"/>
     <col min="22" max="23" width="13.7109375" style="1" customWidth="1"/>
-    <col min="24" max="24" width="12.85546875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="15.7109375" style="1" customWidth="1"/>
-    <col min="26" max="27" width="18" style="1" customWidth="1"/>
-    <col min="28" max="28" width="11.42578125" style="1" customWidth="1"/>
-    <col min="29" max="29" width="17.42578125" style="1" customWidth="1"/>
-    <col min="30" max="31" width="11.28515625" style="1" customWidth="1"/>
-    <col min="32" max="32" width="21" style="1" customWidth="1"/>
-    <col min="33" max="33" width="22" style="1" customWidth="1"/>
-    <col min="34" max="34" width="21" style="1" customWidth="1"/>
-    <col min="35" max="35" width="20.85546875" style="1" customWidth="1"/>
-    <col min="36" max="36" width="37.7109375" style="1" customWidth="1"/>
-    <col min="37" max="37" width="24" style="1" customWidth="1"/>
-    <col min="38" max="16384" width="9.140625" style="1"/>
+    <col min="24" max="25" width="12.85546875" style="1" customWidth="1"/>
+    <col min="26" max="26" width="14.5703125" style="1" customWidth="1"/>
+    <col min="27" max="28" width="12.85546875" style="1" customWidth="1"/>
+    <col min="29" max="29" width="15.7109375" style="1" customWidth="1"/>
+    <col min="30" max="31" width="18" style="1" customWidth="1"/>
+    <col min="32" max="32" width="11.42578125" style="1" customWidth="1"/>
+    <col min="33" max="33" width="17.42578125" style="1" customWidth="1"/>
+    <col min="34" max="35" width="11.28515625" style="1" customWidth="1"/>
+    <col min="36" max="36" width="21" style="1" customWidth="1"/>
+    <col min="37" max="37" width="22" style="1" customWidth="1"/>
+    <col min="38" max="38" width="21" style="1" customWidth="1"/>
+    <col min="39" max="39" width="20.85546875" style="1" customWidth="1"/>
+    <col min="40" max="40" width="37.7109375" style="1" customWidth="1"/>
+    <col min="41" max="41" width="24" style="1" customWidth="1"/>
+    <col min="42" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:41" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>32</v>
       </c>
@@ -1148,8 +1174,12 @@
       <c r="AI1" s="27"/>
       <c r="AJ1" s="27"/>
       <c r="AK1" s="27"/>
+      <c r="AL1" s="27"/>
+      <c r="AM1" s="27"/>
+      <c r="AN1" s="27"/>
+      <c r="AO1" s="27"/>
     </row>
-    <row r="2" spans="1:37" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
@@ -1171,7 +1201,7 @@
       <c r="S2" s="25"/>
       <c r="T2" s="25"/>
     </row>
-    <row r="3" spans="1:37" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
@@ -1245,46 +1275,58 @@
         <v>64</v>
       </c>
       <c r="Y3" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z3" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA3" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB3" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC3" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="Z3" s="9" t="s">
+      <c r="AD3" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="AA3" s="9" t="s">
+      <c r="AE3" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="AB3" s="9" t="s">
+      <c r="AF3" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="AC3" s="9" t="s">
+      <c r="AG3" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="AD3" s="9" t="s">
+      <c r="AH3" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="AE3" s="9" t="s">
+      <c r="AI3" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="AF3" s="9" t="s">
+      <c r="AJ3" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="AG3" s="9" t="s">
+      <c r="AK3" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="AH3" s="9" t="s">
+      <c r="AL3" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="AI3" s="9" t="s">
+      <c r="AM3" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="AJ3" s="9" t="s">
+      <c r="AN3" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="AK3" s="9" t="s">
+      <c r="AO3" s="9" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -1356,46 +1398,58 @@
         <v>63</v>
       </c>
       <c r="Y4" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z4" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA4" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC4" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="Z4" s="7" t="s">
+      <c r="AD4" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AA4" s="7" t="s">
+      <c r="AE4" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="AB4" s="7" t="s">
+      <c r="AF4" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="AC4" s="7" t="s">
+      <c r="AG4" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="AD4" s="7" t="s">
+      <c r="AH4" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AE4" s="7" t="s">
+      <c r="AI4" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="AF4" s="7" t="s">
+      <c r="AJ4" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="AG4" s="7" t="s">
+      <c r="AK4" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="AH4" s="7" t="s">
+      <c r="AL4" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="AI4" s="7" t="s">
+      <c r="AM4" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="AJ4" s="7" t="s">
+      <c r="AN4" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="AK4" s="10" t="s">
+      <c r="AO4" s="10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
@@ -1459,26 +1513,38 @@
       </c>
       <c r="X5" s="10"/>
       <c r="Y5" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA5" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC5" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="Z5" s="10" t="s">
+      <c r="AD5" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="AA5" s="10" t="s">
+      <c r="AE5" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="AB5" s="10"/>
-      <c r="AC5" s="10"/>
-      <c r="AD5" s="10"/>
-      <c r="AE5" s="10"/>
       <c r="AF5" s="10"/>
       <c r="AG5" s="10"/>
       <c r="AH5" s="10"/>
       <c r="AI5" s="10"/>
       <c r="AJ5" s="10"/>
       <c r="AK5" s="10"/>
+      <c r="AL5" s="10"/>
+      <c r="AM5" s="10"/>
+      <c r="AN5" s="10"/>
+      <c r="AO5" s="10"/>
     </row>
-    <row r="6" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>89</v>
       </c>
@@ -1549,47 +1615,59 @@
       <c r="X6" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="Y6" s="23" t="s">
+      <c r="Y6" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB6" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="AC6" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="Z6" s="7" t="s">
+      <c r="AD6" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="AA6" s="7" t="s">
+      <c r="AE6" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="AB6" s="7" t="s">
+      <c r="AF6" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="AC6" s="7" t="s">
+      <c r="AG6" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="AD6" s="7" t="s">
+      <c r="AH6" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AE6" s="7" t="s">
+      <c r="AI6" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="AF6" s="7" t="s">
+      <c r="AJ6" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="AG6" s="7" t="s">
+      <c r="AK6" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="AH6" s="7" t="s">
+      <c r="AL6" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="AI6" s="7" t="s">
+      <c r="AM6" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="AJ6" s="7" t="s">
+      <c r="AN6" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="AK6" s="10" t="s">
+      <c r="AO6" s="10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>97</v>
       </c>
@@ -1661,49 +1739,61 @@
         <v>63</v>
       </c>
       <c r="Y7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA7" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC7" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="Z7" s="7" t="s">
+      <c r="AD7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="AA7" s="10" t="s">
+      <c r="AE7" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="AB7" s="7" t="s">
+      <c r="AF7" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="AC7" s="7" t="s">
+      <c r="AG7" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="AD7" s="7" t="s">
+      <c r="AH7" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AE7" s="7" t="s">
+      <c r="AI7" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="AF7" s="7" t="s">
+      <c r="AJ7" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="AG7" s="7" t="s">
+      <c r="AK7" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="AH7" s="7" t="s">
+      <c r="AL7" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="AI7" s="7" t="s">
+      <c r="AM7" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="AJ7" s="7" t="s">
+      <c r="AN7" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="AK7" s="10" t="s">
+      <c r="AO7" s="10" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A1:AK1"/>
+    <mergeCell ref="A1:AO1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cars page - I negative scenarios is added
</commit_message>
<xml_diff>
--- a/src/test/test_data/Booking.xlsx
+++ b/src/test/test_data/Booking.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\Vezba_booking\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F2BFCD-83B2-4C06-B620-845030AB3638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B69DF7-0177-451C-8A85-DEA26FC468A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Flights" sheetId="1" r:id="rId1"/>
     <sheet name="Stays" sheetId="2" r:id="rId2"/>
+    <sheet name="Cars" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Flights!$A$3:$G$3</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="131">
   <si>
     <t>tc_id</t>
   </si>
@@ -309,9 +310,6 @@
     <t>urlCarPage</t>
   </si>
   <si>
-    <t>car</t>
-  </si>
-  <si>
     <t>FL_004</t>
   </si>
   <si>
@@ -409,6 +407,32 @@
   </si>
   <si>
     <t>November 2022 15</t>
+  </si>
+  <si>
+    <t>PickupLocation</t>
+  </si>
+  <si>
+    <t>wrongAges</t>
+  </si>
+  <si>
+    <t>urlCarsPage</t>
+  </si>
+  <si>
+    <t>cars</t>
+  </si>
+  <si>
+    <t>emptyLocatinMessage</t>
+  </si>
+  <si>
+    <t>wrongAgesMessage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Driver needs to be between 18 and 99 years old
+ </t>
+  </si>
+  <si>
+    <t>Please enter a pick-up location</t>
   </si>
 </sst>
 </file>
@@ -482,7 +506,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -522,6 +546,29 @@
         </stop>
       </gradientFill>
     </fill>
+    <fill>
+      <gradientFill degree="90">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="1">
+          <color theme="5" tint="0.40000610370189521"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill degree="90">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="0.5">
+          <color theme="5" tint="0.40000610370189521"/>
+        </stop>
+        <stop position="1">
+          <color theme="0"/>
+        </stop>
+      </gradientFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -716,7 +763,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -763,6 +810,18 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -779,6 +838,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1097,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1AEBA6-E97B-44CC-BE50-33F6B24023CF}">
   <dimension ref="A1:AO7"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,71 +1211,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="26"/>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26"/>
-      <c r="AB1" s="26"/>
-      <c r="AC1" s="26"/>
-      <c r="AD1" s="26"/>
-      <c r="AE1" s="26"/>
-      <c r="AF1" s="26"/>
-      <c r="AG1" s="26"/>
-      <c r="AH1" s="26"/>
-      <c r="AI1" s="26"/>
-      <c r="AJ1" s="26"/>
-      <c r="AK1" s="26"/>
-      <c r="AL1" s="26"/>
-      <c r="AM1" s="26"/>
-      <c r="AN1" s="26"/>
-      <c r="AO1" s="26"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="30"/>
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="30"/>
+      <c r="AO1" s="30"/>
     </row>
     <row r="2" spans="1:41" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
     </row>
     <row r="3" spans="1:41" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -1283,25 +1351,25 @@
         <v>59</v>
       </c>
       <c r="Y3" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z3" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="Z3" s="8" t="s">
+      <c r="AA3" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="AA3" s="8" t="s">
+      <c r="AB3" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="AB3" s="8" t="s">
-        <v>108</v>
-      </c>
       <c r="AC3" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="AD3" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="AD3" s="8" t="s">
-        <v>96</v>
-      </c>
       <c r="AE3" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AF3" s="8" t="s">
         <v>61</v>
@@ -1400,31 +1468,31 @@
         <v>34</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>90</v>
+        <v>126</v>
       </c>
       <c r="X4" s="6" t="s">
         <v>58</v>
       </c>
       <c r="Y4" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Z4" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA4" s="6" t="s">
         <v>110</v>
-      </c>
-      <c r="AA4" s="6" t="s">
-        <v>111</v>
       </c>
       <c r="AB4" s="6" t="s">
         <v>25</v>
       </c>
       <c r="AC4" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AD4" s="6" t="s">
         <v>44</v>
       </c>
       <c r="AE4" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AF4" s="6" t="s">
         <v>71</v>
@@ -1517,29 +1585,29 @@
       <c r="U5" s="4"/>
       <c r="V5" s="9"/>
       <c r="W5" s="9" t="s">
-        <v>90</v>
+        <v>126</v>
       </c>
       <c r="X5" s="9"/>
       <c r="Y5" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Z5" s="9" t="s">
         <v>25</v>
       </c>
       <c r="AA5" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AB5" s="9" t="s">
         <v>25</v>
       </c>
       <c r="AC5" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD5" s="9" t="s">
         <v>31</v>
       </c>
       <c r="AE5" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AF5" s="9"/>
       <c r="AG5" s="9"/>
@@ -1618,7 +1686,7 @@
         <v>34</v>
       </c>
       <c r="W6" s="3" t="s">
-        <v>90</v>
+        <v>126</v>
       </c>
       <c r="X6" s="6" t="s">
         <v>58</v>
@@ -1633,16 +1701,16 @@
         <v>24</v>
       </c>
       <c r="AB6" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AC6" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AD6" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AE6" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AF6" s="6" t="s">
         <v>71</v>
@@ -1677,7 +1745,7 @@
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>44</v>
@@ -1713,13 +1781,13 @@
         <v>52</v>
       </c>
       <c r="M7" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="N7" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="N7" s="4" t="s">
-        <v>114</v>
-      </c>
       <c r="O7" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P7" s="3" t="s">
         <v>52</v>
@@ -1728,20 +1796,20 @@
         <v>56</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S7" s="3" t="s">
         <v>53</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U7" s="4"/>
       <c r="V7" s="3" t="s">
         <v>34</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>90</v>
+        <v>126</v>
       </c>
       <c r="X7" s="6" t="s">
         <v>58</v>
@@ -1753,7 +1821,7 @@
         <v>29</v>
       </c>
       <c r="AA7" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AB7" s="6" t="s">
         <v>29</v>
@@ -1765,7 +1833,7 @@
         <v>21</v>
       </c>
       <c r="AE7" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AF7" s="6" t="s">
         <v>71</v>
@@ -1813,8 +1881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A940F92-832E-4528-BC43-70A9A766E6BC}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1834,20 +1902,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="29"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="33"/>
     </row>
     <row r="2" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22"/>
@@ -1898,10 +1966,10 @@
         <v>82</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>21</v>
@@ -1931,13 +1999,13 @@
         <v>47</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>57</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>31</v>
@@ -1956,7 +2024,7 @@
         <v>34</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L5" s="16" t="s">
         <v>58</v>
@@ -1970,10 +2038,10 @@
         <v>60</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>31</v>
@@ -2006,10 +2074,10 @@
         <v>60</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>31</v>
@@ -2036,16 +2104,16 @@
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>82</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>44</v>
@@ -2066,6 +2134,208 @@
       <c r="K8" s="18" t="s">
         <v>82</v>
       </c>
+      <c r="L8" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A176126E-FCEE-4997-BA28-7546AABD9F56}">
+  <dimension ref="A1:L8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="10" width="13.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="36"/>
+    </row>
+    <row r="2" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="K4" s="14"/>
+      <c r="L4" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="K5" s="14"/>
+      <c r="L5" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="K6" s="14"/>
+      <c r="L6" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="K7" s="14"/>
+      <c r="L7" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="K8" s="18"/>
       <c r="L8" s="20" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
II negative scenarios is added
</commit_message>
<xml_diff>
--- a/src/test/test_data/Booking.xlsx
+++ b/src/test/test_data/Booking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\Vezba_booking\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B69DF7-0177-451C-8A85-DEA26FC468A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AAE794-865C-4342-9634-567DD200C22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Flights" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="132">
   <si>
     <t>tc_id</t>
   </si>
@@ -409,12 +409,6 @@
     <t>November 2022 15</t>
   </si>
   <si>
-    <t>PickupLocation</t>
-  </si>
-  <si>
-    <t>wrongAges</t>
-  </si>
-  <si>
     <t>urlCarsPage</t>
   </si>
   <si>
@@ -427,12 +421,19 @@
     <t>wrongAgesMessage</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Driver needs to be between 18 and 99 years old
- </t>
-  </si>
-  <si>
     <t>Please enter a pick-up location</t>
+  </si>
+  <si>
+    <t>driverAges</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Driver must be aged 18 to 99</t>
   </si>
 </sst>
 </file>
@@ -807,16 +808,16 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1165,7 +1166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1AEBA6-E97B-44CC-BE50-33F6B24023CF}">
   <dimension ref="A1:AO7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1468,7 +1469,7 @@
         <v>34</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="X4" s="6" t="s">
         <v>58</v>
@@ -1585,7 +1586,7 @@
       <c r="U5" s="4"/>
       <c r="V5" s="9"/>
       <c r="W5" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="X5" s="9"/>
       <c r="Y5" s="9" t="s">
@@ -1686,7 +1687,7 @@
         <v>34</v>
       </c>
       <c r="W6" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="X6" s="6" t="s">
         <v>58</v>
@@ -1809,7 +1810,7 @@
         <v>34</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="X7" s="6" t="s">
         <v>58</v>
@@ -2151,16 +2152,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A176126E-FCEE-4997-BA28-7546AABD9F56}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" style="1" customWidth="1"/>
@@ -2188,41 +2189,41 @@
       <c r="L1" s="36"/>
     </row>
     <row r="2" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23"/>
+      <c r="A2" s="25"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>124</v>
-      </c>
-      <c r="F3" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25" t="s">
+      <c r="K3" s="24"/>
+      <c r="L3" s="24" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2230,12 +2231,14 @@
       <c r="A4" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="14"/>
+      <c r="B4" s="14" t="s">
+        <v>129</v>
+      </c>
       <c r="C4" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>129</v>
+        <v>127</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>131</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>45</v>
@@ -2245,7 +2248,7 @@
       <c r="H4" s="15"/>
       <c r="I4" s="14"/>
       <c r="J4" s="14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K4" s="14"/>
       <c r="L4" s="16" t="s">
@@ -2257,17 +2260,23 @@
         <v>47</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="15"/>
+        <v>130</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>103</v>
+      </c>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K5" s="14"/>
       <c r="L5" s="16" t="s">
@@ -2281,15 +2290,21 @@
       <c r="B6" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="15"/>
+      <c r="C6" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>99</v>
+      </c>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K6" s="14"/>
       <c r="L6" s="16" t="s">
@@ -2311,7 +2326,7 @@
       <c r="H7" s="15"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K7" s="14"/>
       <c r="L7" s="16" t="s">
@@ -2333,7 +2348,7 @@
       <c r="H8" s="19"/>
       <c r="I8" s="18"/>
       <c r="J8" s="14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K8" s="18"/>
       <c r="L8" s="20" t="s">

</xml_diff>

<commit_message>
cucumber tests are modified
</commit_message>
<xml_diff>
--- a/src/test/test_data/Booking.xlsx
+++ b/src/test/test_data/Booking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\Vezba_booking\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AAE794-865C-4342-9634-567DD200C22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68D8AAF-89E2-4668-BA89-B6F0371AE5C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Flights" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="131">
   <si>
     <t>tc_id</t>
   </si>
@@ -307,18 +307,12 @@
     <t>Skopje</t>
   </si>
   <si>
-    <t>urlCarPage</t>
-  </si>
-  <si>
     <t>FL_004</t>
   </si>
   <si>
     <t>Wed 30 Nov</t>
   </si>
   <si>
-    <t>Fri 25 Nov</t>
-  </si>
-  <si>
     <t>TC_005</t>
   </si>
   <si>
@@ -434,6 +428,9 @@
   </si>
   <si>
     <t>Driver must be aged 18 to 99</t>
+  </si>
+  <si>
+    <t>Mon 28 Nov</t>
   </si>
 </sst>
 </file>
@@ -1166,8 +1163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1AEBA6-E97B-44CC-BE50-33F6B24023CF}">
   <dimension ref="A1:AO7"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,7 +1186,7 @@
     <col min="15" max="15" width="15.140625" style="1" customWidth="1"/>
     <col min="16" max="16" width="16.42578125" style="1" customWidth="1"/>
     <col min="17" max="17" width="13.42578125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="1"/>
+    <col min="18" max="18" width="15.28515625" style="1" customWidth="1"/>
     <col min="19" max="19" width="13.28515625" style="1" customWidth="1"/>
     <col min="20" max="20" width="10.28515625" style="1" customWidth="1"/>
     <col min="21" max="21" width="13.85546875" style="1" customWidth="1"/>
@@ -1346,31 +1343,31 @@
         <v>51</v>
       </c>
       <c r="W3" s="8" t="s">
-        <v>89</v>
+        <v>121</v>
       </c>
       <c r="X3" s="8" t="s">
         <v>59</v>
       </c>
       <c r="Y3" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z3" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA3" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="Z3" s="8" t="s">
+      <c r="AB3" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="AA3" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="AB3" s="8" t="s">
-        <v>107</v>
-      </c>
       <c r="AC3" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AD3" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AE3" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AF3" s="8" t="s">
         <v>61</v>
@@ -1469,31 +1466,31 @@
         <v>34</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="X4" s="6" t="s">
         <v>58</v>
       </c>
       <c r="Y4" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="Z4" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AA4" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AB4" s="6" t="s">
         <v>25</v>
       </c>
       <c r="AC4" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AD4" s="6" t="s">
         <v>44</v>
       </c>
       <c r="AE4" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AF4" s="6" t="s">
         <v>71</v>
@@ -1569,14 +1566,18 @@
       <c r="N5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="O5" s="4"/>
+      <c r="O5" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="P5" s="3" t="s">
         <v>52</v>
       </c>
       <c r="Q5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="R5" s="3"/>
+      <c r="R5" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="S5" s="3" t="s">
         <v>53</v>
       </c>
@@ -1586,29 +1587,29 @@
       <c r="U5" s="4"/>
       <c r="V5" s="9"/>
       <c r="W5" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="X5" s="9"/>
       <c r="Y5" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="Z5" s="9" t="s">
         <v>25</v>
       </c>
       <c r="AA5" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AB5" s="9" t="s">
         <v>25</v>
       </c>
       <c r="AC5" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AD5" s="9" t="s">
         <v>31</v>
       </c>
       <c r="AE5" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AF5" s="9"/>
       <c r="AG5" s="9"/>
@@ -1687,7 +1688,7 @@
         <v>34</v>
       </c>
       <c r="W6" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="X6" s="6" t="s">
         <v>58</v>
@@ -1702,16 +1703,16 @@
         <v>24</v>
       </c>
       <c r="AB6" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AC6" s="21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="AD6" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AE6" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AF6" s="6" t="s">
         <v>71</v>
@@ -1746,7 +1747,7 @@
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>44</v>
@@ -1782,13 +1783,13 @@
         <v>52</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>92</v>
+        <v>130</v>
       </c>
       <c r="P7" s="3" t="s">
         <v>52</v>
@@ -1797,20 +1798,20 @@
         <v>56</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="S7" s="3" t="s">
         <v>53</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="U7" s="4"/>
       <c r="V7" s="3" t="s">
         <v>34</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="X7" s="6" t="s">
         <v>58</v>
@@ -1822,7 +1823,7 @@
         <v>29</v>
       </c>
       <c r="AA7" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AB7" s="6" t="s">
         <v>29</v>
@@ -1834,7 +1835,7 @@
         <v>21</v>
       </c>
       <c r="AE7" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="AF7" s="6" t="s">
         <v>71</v>
@@ -1967,10 +1968,10 @@
         <v>82</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>21</v>
@@ -2000,13 +2001,13 @@
         <v>47</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>57</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>31</v>
@@ -2025,7 +2026,7 @@
         <v>34</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L5" s="16" t="s">
         <v>58</v>
@@ -2039,10 +2040,10 @@
         <v>60</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>31</v>
@@ -2075,10 +2076,10 @@
         <v>60</v>
       </c>
       <c r="C7" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>118</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>120</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>31</v>
@@ -2105,16 +2106,16 @@
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>82</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>44</v>
@@ -2150,10 +2151,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A176126E-FCEE-4997-BA28-7546AABD9F56}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2164,15 +2165,15 @@
     <col min="4" max="4" width="29.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="10" width="13.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="8" width="13.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10" max="11" width="13.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="34" t="s">
         <v>32</v>
       </c>
@@ -2186,12 +2187,13 @@
       <c r="I1" s="35"/>
       <c r="J1" s="35"/>
       <c r="K1" s="35"/>
-      <c r="L1" s="36"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="36"/>
     </row>
-    <row r="2" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="25"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>0</v>
       </c>
@@ -2199,91 +2201,112 @@
         <v>2</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D3" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="E3" s="24" t="s">
-        <v>128</v>
-      </c>
       <c r="F3" s="24" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>41</v>
+        <v>104</v>
       </c>
       <c r="I3" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="J3" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24" t="s">
+      <c r="K3" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>46</v>
       </c>
       <c r="B4" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>129</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>131</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="K4" s="14"/>
-      <c r="L4" s="16" t="s">
+      <c r="F4" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="L4" s="14"/>
+      <c r="M4" s="16" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>47</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="K5" s="14"/>
-      <c r="L5" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="L5" s="14"/>
+      <c r="M5" s="16" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>48</v>
       </c>
@@ -2291,27 +2314,36 @@
         <v>60</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="K6" s="14"/>
-      <c r="L6" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="L6" s="14"/>
+      <c r="M6" s="16" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>49</v>
       </c>
@@ -2324,18 +2356,19 @@
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="K7" s="14"/>
-      <c r="L7" s="16" t="s">
+      <c r="I7" s="15"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="L7" s="14"/>
+      <c r="M7" s="16" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>82</v>
@@ -2346,18 +2379,19 @@
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
       <c r="H8" s="19"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="K8" s="18"/>
-      <c r="L8" s="20" t="s">
+      <c r="I8" s="19"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="L8" s="18"/>
+      <c r="M8" s="20" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>